<commit_message>
Adding Top100 based on NPR
</commit_message>
<xml_diff>
--- a/HSData/Data/2017top100HS_1014_mapping.xlsx
+++ b/HSData/Data/2017top100HS_1014_mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HSData\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\HMAResearch\HSData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{34319C99-7276-45B9-BBB7-CEBA24667E97}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D13938CD-DC84-4558-AB2A-3B39F69CB7EC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$G$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$G$101</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
@@ -1292,7 +1292,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2912,7 +2912,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G100" xr:uid="{5F738141-BCEE-4E24-B98D-EA3F52F5890E}"/>
+  <autoFilter ref="A1:G101" xr:uid="{5F738141-BCEE-4E24-B98D-EA3F52F5890E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>